<commit_message>
Add parsing all tables with indicators
</commit_message>
<xml_diff>
--- a/Data/Russian_Universities_Initial.xlsx
+++ b/Data/Russian_Universities_Initial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/educauchy/Google Drive/Университет/Магистратура/Research/Programs/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA08269E-4C22-B04A-BAE8-543A9C54FDA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E013FF2-146F-7141-8C9C-5E6272000DED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6540" windowWidth="28800" windowHeight="11460" xr2:uid="{51EEAB5F-437A-7443-B49F-6569084985F9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{51EEAB5F-437A-7443-B49F-6569084985F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B5B4B-573F-B842-BA0F-08A572ABB545}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>